<commit_message>
added third sheet to excel
</commit_message>
<xml_diff>
--- a/01. Proiect_vacation_rate_repo/Vacation_rate_v2/VacationRate.xlsx
+++ b/01. Proiect_vacation_rate_repo/Vacation_rate_v2/VacationRate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldobre2\Desktop\vacationRate_Repo\VacationRate\01. Proiect_vacation_rate_repo\Vacation_rate_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CC86FC-86D0-4885-8B92-80AEADED3A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD967D66-2E1B-418E-B0B1-7A13DB5FAA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="2412" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Absences" sheetId="1" r:id="rId1"/>
@@ -90650,7 +90650,7 @@
   <dimension ref="A1:D383"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>